<commit_message>
FEATURE: Fecth Busince Confidence file from INE
</commit_message>
<xml_diff>
--- a/src/businessConfidenceAggregate/assets/report.xlsx
+++ b/src/businessConfidenceAggregate/assets/report.xlsx
@@ -19,7 +19,7 @@
     <t>Atualização dos Índices Agregados do Volume de Negócios: Relatório da Ultima actividade</t>
   </si>
   <si>
-    <t>Task Code</t>
+    <t>Job Code</t>
   </si>
   <si>
     <t>Name</t>
@@ -43,13 +43,13 @@
     <t>Economic Activity Index</t>
   </si>
   <si>
-    <t>Economic Activity Index update</t>
+    <t>Economic Activity update</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>aggregate Economic Activities: has a format error on energia,água e san</t>
+    <t>Could not fetch the Economic Activities Index, the url is http://www.ine.gov.mz/estatisticas/estatisticas-economicas/icce</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>44829.4252286966</v>
+        <v>44831.64273728427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEATURE: Create Schedule to update Business Confidence
</commit_message>
<xml_diff>
--- a/src/businessConfidenceAggregate/assets/report.xlsx
+++ b/src/businessConfidenceAggregate/assets/report.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>Atualização dos Índices Agregados do Volume de Negócios: Relatório da Ultima actividade</t>
+    <t>Atualização dos Indicadores de Confiança e de Clima Económico: Relatório da Ultima actividade</t>
   </si>
   <si>
     <t>Job Code</t>
@@ -40,10 +40,10 @@
     <t>04-job</t>
   </si>
   <si>
-    <t>Economic Activity Index</t>
-  </si>
-  <si>
-    <t>Economic Activity update</t>
+    <t>Aggregate Business Confidence</t>
+  </si>
+  <si>
+    <t>Aggregate Business Confidence update</t>
   </si>
   <si>
     <t>No</t>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>44831.64273728427</v>
+        <v>44831.67255092743</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEATURE: Download Business Confidence PDF file
</commit_message>
<xml_diff>
--- a/src/businessConfidenceAggregate/assets/report.xlsx
+++ b/src/businessConfidenceAggregate/assets/report.xlsx
@@ -49,7 +49,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Could not fetch the Economic Activities Index, the url is http://www.ine.gov.mz/estatisticas/estatisticas-economicas/icce</t>
+    <t>Could not fetch the Economic Activities Index, the url is http://www.ine.gov.mz/estatisticas/estatisticas-economicas/icce/icce-t1-2022-_v2jr.pdf</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>44831.67255092743</v>
+        <v>44832.5362676465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEATURE: Download Economic Activity
</commit_message>
<xml_diff>
--- a/src/businessConfidenceAggregate/assets/report.xlsx
+++ b/src/businessConfidenceAggregate/assets/report.xlsx
@@ -49,7 +49,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Could not fetch the Economic Activities Index, the url is http://www.ine.gov.mz/estatisticas/estatisticas-economicas/icce/icce-t1-2022-_v2jr.pdf</t>
+    <t>Could not download the pdf file, the url is http://www.ine.gov.mz/estatisticas/estatisticas-economicas/indice-de-actividades-economicas-iae/brochura_iae_no216-marco-2022.pdf</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>44832.5362676465</v>
+        <v>44832.69050239767</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IMPROVE: Economic Activity Data Extract
</commit_message>
<xml_diff>
--- a/src/businessConfidenceAggregate/assets/report.xlsx
+++ b/src/businessConfidenceAggregate/assets/report.xlsx
@@ -49,7 +49,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Could not download the pdf file, the url is http://www.ine.gov.mz/estatisticas/estatisticas-economicas/indice-de-actividades-economicas-iae/brochura_iae_no216-marco-2022.pdf</t>
+    <t>Could not download the pdf file, the url is http://www.ine.gov.mz/estatisticas/estatisticas-economicas/indice-de-actividades-economicas-iae/indices-de-actividades-economicas_iae_no220-julho_-2022.pdf</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>44833.84911540788</v>
+        <v>44834.86281814193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEATURE: Business Confidece Data
</commit_message>
<xml_diff>
--- a/src/businessConfidenceAggregate/assets/report.xlsx
+++ b/src/businessConfidenceAggregate/assets/report.xlsx
@@ -49,7 +49,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>aggregate Economic Activities Index: has a format error on aloj.rest. similares</t>
+    <t>The business-confidence-aggregate table could not be filtered. Error occurred</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>44835.13390795871</v>
+        <v>44836.63922199089</v>
       </c>
     </row>
   </sheetData>

</xml_diff>